<commit_message>
dividing data into different categories
</commit_message>
<xml_diff>
--- a/data/affiliations_wos.xlsx
+++ b/data/affiliations_wos.xlsx
@@ -393,7 +393,7 @@
         <v>CHINESE ACADEMY OF SCIENCES</v>
       </c>
       <c r="B2">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3">
@@ -409,7 +409,7 @@
         <v>UNIVERSITY OF CHINESE ACADEMY OF SCIENCES CAS</v>
       </c>
       <c r="B4">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5">
@@ -417,7 +417,7 @@
         <v>SOUTH CHINA UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B5">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6">
@@ -430,50 +430,50 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>HARBIN INSTITUTE OF TECHNOLOGY</v>
+        <v>DELFT UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B7">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>DELFT UNIVERSITY OF TECHNOLOGY</v>
+        <v>SOUTHEAST UNIVERSITY CHINA</v>
       </c>
       <c r="B8">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>SOUTHEAST UNIVERSITY CHINA</v>
+        <v>HARBIN INSTITUTE OF TECHNOLOGY</v>
       </c>
       <c r="B9">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>TSINGHUA UNIVERSITY</v>
+        <v>WUHAN UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B10">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>NANJING FORESTRY UNIVERSITY</v>
+        <v>TSINGHUA UNIVERSITY</v>
       </c>
       <c r="B11">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>UNIVERSITY OF SCIENCE TECHNOLOGY OF CHINA CAS</v>
+        <v>NANJING FORESTRY UNIVERSITY</v>
       </c>
       <c r="B12">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13">
@@ -481,95 +481,95 @@
         <v>SHENZHEN UNIVERSITY</v>
       </c>
       <c r="B13">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>UNITED STATES DEPARTMENT OF ENERGY DOE</v>
+        <v>UNIVERSITY OF SCIENCE TECHNOLOGY OF CHINA CAS</v>
       </c>
       <c r="B14">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>WUHAN UNIVERSITY OF TECHNOLOGY</v>
+        <v>UNITED STATES DEPARTMENT OF ENERGY DOE</v>
       </c>
       <c r="B15">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>NORTHWESTERN POLYTECHNICAL UNIVERSITY</v>
+        <v>TONGJI UNIVERSITY</v>
       </c>
       <c r="B16">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>ZHEJIANG UNIVERSITY</v>
+        <v>NORTHWESTERN POLYTECHNICAL UNIVERSITY</v>
       </c>
       <c r="B17">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>CENTRE NATIONAL DE LA RECHERCHE SCIENTIFIQUE CNRS</v>
+        <v>ZHEJIANG UNIVERSITY</v>
       </c>
       <c r="B18">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>INDIAN INSTITUTE OF TECHNOLOGY SYSTEM IIT SYSTEM</v>
+        <v>CENTRE NATIONAL DE LA RECHERCHE SCIENTIFIQUE CNRS</v>
       </c>
       <c r="B19">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>TONGJI UNIVERSITY</v>
+        <v>GHENT UNIVERSITY</v>
       </c>
       <c r="B20">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>CHONGQING UNIVERSITY</v>
+        <v>INDIAN INSTITUTE OF TECHNOLOGY SYSTEM IIT SYSTEM</v>
       </c>
       <c r="B21">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>HUAZHONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>CHONGQING UNIVERSITY</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>JILIN UNIVERSITY</v>
+        <v>HUAZHONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B23">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>GHENT UNIVERSITY</v>
+        <v>JILIN UNIVERSITY</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
@@ -577,7 +577,7 @@
         <v>UNIVERSITY OF SCIENCE TECHNOLOGY BEIJING</v>
       </c>
       <c r="B25">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -585,7 +585,7 @@
         <v>SUN YAT SEN UNIVERSITY</v>
       </c>
       <c r="B26">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27">
@@ -593,7 +593,7 @@
         <v>NINGBO INSTITUTE OF MATERIALS TECHNOLOGY AND ENGINEERING CAS</v>
       </c>
       <c r="B27">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28">
@@ -601,52 +601,52 @@
         <v>ZHENGZHOU UNIVERSITY</v>
       </c>
       <c r="B28">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>SHANGHAI JIAO TONG UNIVERSITY</v>
+        <v>CHANG AN UNIVERSITY</v>
       </c>
       <c r="B29">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>TIANJIN UNIVERSITY</v>
+        <v>POLYTECHNIC UNIVERSITY OF MILAN</v>
       </c>
       <c r="B30">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>XI AN JIAOTONG UNIVERSITY</v>
+        <v>SHANGHAI JIAO TONG UNIVERSITY</v>
       </c>
       <c r="B31">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>POLYTECHNIC UNIVERSITY OF MILAN</v>
+        <v>XI AN JIAOTONG UNIVERSITY</v>
       </c>
       <c r="B32">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>SHANDONG UNIVERSITY</v>
+        <v>TIANJIN UNIVERSITY</v>
       </c>
       <c r="B33">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>UNIVERSITY OF CALIFORNIA SYSTEM</v>
+        <v>SHANDONG UNIVERSITY</v>
       </c>
       <c r="B34">
         <v>80</v>
@@ -654,87 +654,87 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>CHANG AN UNIVERSITY</v>
+        <v>UNIVERSITY OF CALIFORNIA SYSTEM</v>
       </c>
       <c r="B35">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>SOOCHOW UNIVERSITY CHINA</v>
+        <v>VRIJE UNIVERSITEIT BRUSSEL</v>
       </c>
       <c r="B36">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>NANJING UNIVERSITY</v>
+        <v>SOOCHOW UNIVERSITY CHINA</v>
       </c>
       <c r="B37">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>VRIJE UNIVERSITEIT BRUSSEL</v>
+        <v>DALIAN UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B38">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>UNIVERSITY OF ILLINOIS SYSTEM</v>
+        <v>NANJING UNIVERSITY</v>
       </c>
       <c r="B39">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>CENTRAL SOUTH UNIVERSITY</v>
+        <v>EGYPTIAN KNOWLEDGE BANK EKB</v>
       </c>
       <c r="B40">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>NANYANG TECHNOLOGICAL UNIVERSITY</v>
+        <v>UNIVERSITY OF ILLINOIS SYSTEM</v>
       </c>
       <c r="B41">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>QINGDAO UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>NANYANG TECHNOLOGICAL UNIVERSITY</v>
       </c>
       <c r="B42">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>DALIAN UNIVERSITY OF TECHNOLOGY</v>
+        <v>CENTRAL SOUTH UNIVERSITY</v>
       </c>
       <c r="B43">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>DONGHUA UNIVERSITY</v>
+        <v>QINGDAO UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B44">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>EGYPTIAN KNOWLEDGE BANK EKB</v>
+        <v>DONGHUA UNIVERSITY</v>
       </c>
       <c r="B45">
         <v>72</v>
@@ -745,7 +745,7 @@
         <v>NATIONAL INSTITUTE OF TECHNOLOGY NIT SYSTEM</v>
       </c>
       <c r="B46">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47">
@@ -785,7 +785,7 @@
         <v>NANJING UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B51">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52">
@@ -798,15 +798,15 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>CHINESE ACADEMY OF FORESTRY</v>
+        <v>CONSEJO SUPERIOR DE INVESTIGACIONES CIENTIFICAS CSIC</v>
       </c>
       <c r="B53">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>CONSEJO SUPERIOR DE INVESTIGACIONES CIENTIFICAS CSIC</v>
+        <v>CHINESE ACADEMY OF FORESTRY</v>
       </c>
       <c r="B54">
         <v>63</v>
@@ -814,15 +814,15 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>INST COLOR SCI TECHNOL</v>
+        <v>UNIVERSITY SYSTEM OF OHIO</v>
       </c>
       <c r="B55">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>UNIVERSITY SYSTEM OF OHIO</v>
+        <v>NANJING TECH UNIVERSITY</v>
       </c>
       <c r="B56">
         <v>61</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>NANJING TECH UNIVERSITY</v>
+        <v>INST COLOR SCI TECHNOL</v>
       </c>
       <c r="B57">
         <v>60</v>
@@ -854,15 +854,15 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>FUDAN UNIVERSITY</v>
+        <v>SHANDONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B60">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>SHANDONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>FUDAN UNIVERSITY</v>
       </c>
       <c r="B61">
         <v>58</v>
@@ -881,7 +881,7 @@
         <v>GUANGXI UNIVERSITY</v>
       </c>
       <c r="B63">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64">
@@ -910,31 +910,31 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>COUNCIL OF SCIENTIFIC INDUSTRIAL RESEARCH CSIR INDIA</v>
+        <v>SUNGKYUNKWAN UNIVERSITY SKKU</v>
       </c>
       <c r="B67">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>SUNGKYUNKWAN UNIVERSITY SKKU</v>
+        <v>UNIVERSITY OF CAMBRIDGE</v>
       </c>
       <c r="B68">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>UNIVERSITY OF CAMBRIDGE</v>
+        <v>UNIVERSITY SYSTEM OF GEORGIA</v>
       </c>
       <c r="B69">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>UNIVERSITY SYSTEM OF GEORGIA</v>
+        <v>COUNCIL OF SCIENTIFIC INDUSTRIAL RESEARCH CSIR INDIA</v>
       </c>
       <c r="B70">
         <v>53</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>OCEAN UNIVERSITY OF CHINA</v>
+        <v>KOREA UNIVERSITY</v>
       </c>
       <c r="B72">
         <v>51</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>UNIVERSITY OF ELECTRONIC SCIENCE TECHNOLOGY OF CHINA</v>
+        <v>OCEAN UNIVERSITY OF CHINA</v>
       </c>
       <c r="B73">
         <v>51</v>
@@ -966,23 +966,23 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>KOREA UNIVERSITY</v>
+        <v>UNIVERSITY OF ELECTRONIC SCIENCE TECHNOLOGY OF CHINA</v>
       </c>
       <c r="B74">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>GUANGDONG UNIVERSITY OF TECHNOLOGY</v>
+        <v>BEIHANG UNIVERSITY</v>
       </c>
       <c r="B75">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>NANJING UNIVERSITY OF AERONAUTICS ASTRONAUTICS</v>
+        <v>GUANGDONG UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B76">
         <v>49</v>
@@ -990,18 +990,18 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>BEIHANG UNIVERSITY</v>
+        <v>INSTITUTE OF OCEANOLOGY CAS</v>
       </c>
       <c r="B77">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>INSTITUTE OF OCEANOLOGY CAS</v>
+        <v>NANJING UNIVERSITY OF AERONAUTICS ASTRONAUTICS</v>
       </c>
       <c r="B78">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79">
@@ -1022,87 +1022,87 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>CITY UNIVERSITY OF HONG KONG</v>
+        <v>LOUISIANA STATE UNIVERSITY</v>
       </c>
       <c r="B81">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>HANYANG UNIVERSITY</v>
+        <v>LOUISIANA STATE UNIVERSITY SYSTEM</v>
       </c>
       <c r="B82">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>UNIVERSITY OF MICHIGAN</v>
+        <v>HANYANG UNIVERSITY</v>
       </c>
       <c r="B83">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>UNIVERSITY OF MICHIGAN SYSTEM</v>
+        <v>HONG KONG POLYTECHNIC UNIVERSITY</v>
       </c>
       <c r="B84">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>GEORGIA INSTITUTE OF TECHNOLOGY</v>
+        <v>CITY UNIVERSITY OF HONG KONG</v>
       </c>
       <c r="B85">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>HONG KONG POLYTECHNIC UNIVERSITY</v>
+        <v>GEORGIA INSTITUTE OF TECHNOLOGY</v>
       </c>
       <c r="B86">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>UNIVERSITY OF TEXAS SYSTEM</v>
+        <v>HEBEI UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B87">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>HEBEI UNIVERSITY OF TECHNOLOGY</v>
+        <v>UNIVERSITY OF MICHIGAN</v>
       </c>
       <c r="B88">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>INSTITUTE OF METAL RESEARCH CAS</v>
+        <v>UNIVERSITY OF MICHIGAN SYSTEM</v>
       </c>
       <c r="B89">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>LOUISIANA STATE UNIVERSITY</v>
+        <v>UNIVERSITY OF TEXAS SYSTEM</v>
       </c>
       <c r="B90">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>LOUISIANA STATE UNIVERSITY SYSTEM</v>
+        <v>INSTITUTE OF METAL RESEARCH CAS</v>
       </c>
       <c r="B91">
         <v>43</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>TIANGONG UNIVERSITY</v>
+        <v>PENNSYLVANIA COMMONWEALTH SYSTEM OF HIGHER EDUCATION PCSHE</v>
       </c>
       <c r="B94">
         <v>42</v>
@@ -1134,15 +1134,15 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>CHANGCHUN INSTITUTE OF APPLIED CHEMISTRY CAS</v>
+        <v>TIANGONG UNIVERSITY</v>
       </c>
       <c r="B95">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>MONASH UNIVERSITY</v>
+        <v>CHANGCHUN INSTITUTE OF APPLIED CHEMISTRY CAS</v>
       </c>
       <c r="B96">
         <v>41</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>PENNSYLVANIA COMMONWEALTH SYSTEM OF HIGHER EDUCATION PCSHE</v>
+        <v>MONASH UNIVERSITY</v>
       </c>
       <c r="B97">
         <v>41</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>QINGDAO UNIVERSITY</v>
+        <v>NORTHEAST FORESTRY UNIVERSITY CHINA</v>
       </c>
       <c r="B99">
         <v>40</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>STATE UNIVERSITY SYSTEM OF FLORIDA</v>
+        <v>QINGDAO UNIVERSITY</v>
       </c>
       <c r="B100">
         <v>40</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>UNIVERSITY OF WISCONSIN SYSTEM</v>
+        <v>STATE UNIVERSITY SYSTEM OF FLORIDA</v>
       </c>
       <c r="B101">
         <v>40</v>
@@ -1190,15 +1190,15 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>CONSIGLIO NAZIONALE DELLE RICERCHE CNR</v>
+        <v>UNIVERSITY OF WISCONSIN SYSTEM</v>
       </c>
       <c r="B102">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>GUILIN UNIVERSITY OF TECHNOLOGY</v>
+        <v>CONSIGLIO NAZIONALE DELLE RICERCHE CNR</v>
       </c>
       <c r="B103">
         <v>39</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>MARTIN LUTHER UNIVERSITY HALLE WITTENBERG</v>
+        <v>GUILIN UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B104">
         <v>39</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>NORTHEAST FORESTRY UNIVERSITY CHINA</v>
+        <v>MARTIN LUTHER UNIVERSITY HALLE WITTENBERG</v>
       </c>
       <c r="B105">
         <v>39</v>
@@ -1246,23 +1246,23 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>HUNAN UNIVERSITY</v>
+        <v>TEXAS A M UNIVERSITY SYSTEM</v>
       </c>
       <c r="B109">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>TEXAS A M UNIVERSITY SYSTEM</v>
+        <v>UNIVERSITY OF TOKYO</v>
       </c>
       <c r="B110">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>UNIVERSITY OF TOKYO</v>
+        <v>HUNAN UNIVERSITY</v>
       </c>
       <c r="B111">
         <v>38</v>
@@ -1270,15 +1270,15 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>FUZHOU UNIVERSITY</v>
+        <v>ISFAHAN UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B112">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>SEOUL NATIONAL UNIVERSITY SNU</v>
+        <v>FUZHOU UNIVERSITY</v>
       </c>
       <c r="B113">
         <v>37</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>YONSEI UNIVERSITY</v>
+        <v>SEOUL NATIONAL UNIVERSITY SNU</v>
       </c>
       <c r="B114">
         <v>37</v>
@@ -1294,15 +1294,15 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>FRIEDRICH SCHILLER UNIVERSITY OF JENA</v>
+        <v>YONSEI UNIVERSITY</v>
       </c>
       <c r="B115">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>ISFAHAN UNIVERSITY OF TECHNOLOGY</v>
+        <v>FRIEDRICH SCHILLER UNIVERSITY OF JENA</v>
       </c>
       <c r="B116">
         <v>36</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>KOREA RESEARCH INSTITUTE OF CHEMICAL TECHNOLOGY KRICT</v>
+        <v>JIANGSU UNIVERSITY</v>
       </c>
       <c r="B117">
         <v>36</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>SHENZHEN INSTITUTE OF ADVANCED TECHNOLOGY CAS</v>
+        <v>KOREA RESEARCH INSTITUTE OF CHEMICAL TECHNOLOGY KRICT</v>
       </c>
       <c r="B118">
         <v>36</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>UNIVERSITY OF TENNESSEE KNOXVILLE</v>
+        <v>NORTHWESTERN UNIVERSITY</v>
       </c>
       <c r="B119">
         <v>36</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>UNIVERSITY OF TENNESSEE SYSTEM</v>
+        <v>SHENZHEN INSTITUTE OF ADVANCED TECHNOLOGY CAS</v>
       </c>
       <c r="B120">
         <v>36</v>
@@ -1342,31 +1342,31 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>JIANGSU UNIVERSITY</v>
+        <v>TEXAS A M UNIVERSITY COLLEGE STATION</v>
       </c>
       <c r="B121">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>NORTHWESTERN UNIVERSITY</v>
+        <v>UNIVERSITY OF TENNESSEE KNOXVILLE</v>
       </c>
       <c r="B122">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>PENNSYLVANIA STATE UNIVERSITY</v>
+        <v>UNIVERSITY OF TENNESSEE SYSTEM</v>
       </c>
       <c r="B123">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>SHANGHAI UNIVERSITY</v>
+        <v>NORTHEASTERN UNIVERSITY CHINA</v>
       </c>
       <c r="B124">
         <v>35</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>TEXAS A M UNIVERSITY COLLEGE STATION</v>
+        <v>PENNSYLVANIA STATE UNIVERSITY</v>
       </c>
       <c r="B125">
         <v>35</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>UNIVERSITY OF LONDON</v>
+        <v>POLYTECHNIC UNIVERSITY OF TURIN</v>
       </c>
       <c r="B126">
         <v>35</v>
@@ -1390,39 +1390,39 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>POLYTECHNIC UNIVERSITY OF TURIN</v>
+        <v>SHANGHAI UNIVERSITY</v>
       </c>
       <c r="B127">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>INDIAN INSTITUTE OF TECHNOLOGY IIT KHARAGPUR</v>
+        <v>UNIVERSITY OF LONDON</v>
       </c>
       <c r="B128">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>NORTHEASTERN UNIVERSITY CHINA</v>
+        <v>JIANGSU UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B129">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>PENNSYLVANIA STATE UNIVERSITY UNIVERSITY PARK</v>
+        <v>SOUTHWEST JIAOTONG UNIVERSITY</v>
       </c>
       <c r="B130">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>SOUTHWEST JIAOTONG UNIVERSITY</v>
+        <v>INDIAN INSTITUTE OF TECHNOLOGY IIT KHARAGPUR</v>
       </c>
       <c r="B131">
         <v>33</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>STANFORD UNIVERSITY</v>
+        <v>PENNSYLVANIA STATE UNIVERSITY UNIVERSITY PARK</v>
       </c>
       <c r="B132">
         <v>33</v>
@@ -1438,31 +1438,31 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>INSTITUTE OF CHEMISTRY CAS</v>
+        <v>STANFORD UNIVERSITY</v>
       </c>
       <c r="B133">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>CNRS INSTITUTE OF CHEMISTRY INC</v>
+        <v>INSTITUTE OF CHEMISTRY CAS</v>
       </c>
       <c r="B134">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>HONG KONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>WUHAN UNIVERSITY</v>
       </c>
       <c r="B135">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>HUBEI UNIVERSITY</v>
+        <v>CNRS INSTITUTE OF CHEMISTRY INC</v>
       </c>
       <c r="B136">
         <v>31</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>JIANGSU UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>HARBIN ENGINEERING UNIVERSITY</v>
       </c>
       <c r="B137">
         <v>31</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>KING SAUD UNIVERSITY</v>
+        <v>HONG KONG UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B138">
         <v>31</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>UNIVERSITY OF BASQUE COUNTRY</v>
+        <v>HUBEI UNIVERSITY</v>
       </c>
       <c r="B139">
         <v>31</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>UNIVERSITY OF TORONTO</v>
+        <v>KING SAUD UNIVERSITY</v>
       </c>
       <c r="B140">
         <v>31</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>WUHAN UNIVERSITY</v>
+        <v>NINGBO UNIVERSITY</v>
       </c>
       <c r="B141">
         <v>31</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>XIAMEN UNIVERSITY</v>
+        <v>UNIVERSITY OF BASQUE COUNTRY</v>
       </c>
       <c r="B142">
         <v>31</v>
@@ -1518,23 +1518,23 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>CARDIFF UNIVERSITY</v>
+        <v>UNIVERSITY OF TORONTO</v>
       </c>
       <c r="B143">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>EAST CHINA UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>XIAMEN UNIVERSITY</v>
       </c>
       <c r="B144">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>NINGBO UNIVERSITY</v>
+        <v>CARDIFF UNIVERSITY</v>
       </c>
       <c r="B145">
         <v>30</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>SOUTHERN UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>EAST CHINA UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B146">
         <v>30</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>UNIVERSITY OF PETROLEUM ENERGY STUDIES UPES</v>
+        <v>SOUTHERN UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B147">
         <v>30</v>
@@ -1558,15 +1558,15 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>CHINESE ACADEMY OF ENGINEERING PHYSICS</v>
+        <v>UNIVERSITY OF PETROLEUM ENERGY STUDIES UPES</v>
       </c>
       <c r="B148">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>ECOLE POLYTECHNIQUE FEDERALE DE LAUSANNE</v>
+        <v>CHINESE ACADEMY OF ENGINEERING PHYSICS</v>
       </c>
       <c r="B149">
         <v>29</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>HARBIN ENGINEERING UNIVERSITY</v>
+        <v>ECOLE POLYTECHNIQUE FEDERALE DE LAUSANNE</v>
       </c>
       <c r="B150">
         <v>29</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>UNIVERSITI SAINS MALAYSIA</v>
+        <v>TAIYUAN UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B152">
         <v>29</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>UNIVERSITY OF WISCONSIN MILWAUKEE</v>
+        <v>UNIVERSITI SAINS MALAYSIA</v>
       </c>
       <c r="B153">
         <v>29</v>
@@ -1606,23 +1606,23 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>NANKAI UNIVERSITY</v>
+        <v>UNIVERSITY OF BATH</v>
       </c>
       <c r="B154">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>ULSAN NATIONAL INSTITUTE OF SCIENCE TECHNOLOGY UNIST</v>
+        <v>UNIVERSITY OF WISCONSIN MILWAUKEE</v>
       </c>
       <c r="B155">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>UNITED STATES DEPARTMENT OF DEFENSE</v>
+        <v>KU LEUVEN</v>
       </c>
       <c r="B156">
         <v>28</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>UNIVERSITY OF COLORADO SYSTEM</v>
+        <v>NANCHANG UNIVERSITY</v>
       </c>
       <c r="B157">
         <v>28</v>
@@ -1638,39 +1638,39 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>AGENCY FOR SCIENCE TECHNOLOGY RESEARCH A STAR</v>
+        <v>NANKAI UNIVERSITY</v>
       </c>
       <c r="B158">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>MINIST EDUC</v>
+        <v>ULSAN NATIONAL INSTITUTE OF SCIENCE TECHNOLOGY UNIST</v>
       </c>
       <c r="B159">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>NANCHANG UNIVERSITY</v>
+        <v>UNITED STATES DEPARTMENT OF DEFENSE</v>
       </c>
       <c r="B160">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>UNIVERSITY OF BATH</v>
+        <v>UNIVERSITY OF COLORADO SYSTEM</v>
       </c>
       <c r="B161">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>UNIVERSITY OF TEHRAN</v>
+        <v>AGENCY FOR SCIENCE TECHNOLOGY RESEARCH A STAR</v>
       </c>
       <c r="B162">
         <v>27</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>WUHAN TEXTILE UNIVERSITY</v>
+        <v>CHINA UNIVERSITY OF GEOSCIENCES</v>
       </c>
       <c r="B163">
         <v>27</v>
@@ -1686,63 +1686,63 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>CHANGZHOU UNIVERSITY</v>
+        <v>MINIST EDUC</v>
       </c>
       <c r="B164">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>ETH ZURICH</v>
+        <v>NORTH CAROLINA STATE UNIVERSITY</v>
       </c>
       <c r="B165">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>KING FAHD UNIVERSITY OF PETROLEUM MINERALS</v>
+        <v>QINGDAO UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B166">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>NORTH CAROLINA STATE UNIVERSITY</v>
+        <v>UNIVERSIDAD DEL BIO BIO</v>
       </c>
       <c r="B167">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>QINGDAO UNIVERSITY OF TECHNOLOGY</v>
+        <v>UNIVERSITY OF TEHRAN</v>
       </c>
       <c r="B168">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>UNIVERSITE DE MONTREAL</v>
+        <v>WUHAN TEXTILE UNIVERSITY</v>
       </c>
       <c r="B169">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>UNIVERSITY OF GRONINGEN</v>
+        <v>YANGZHOU UNIVERSITY</v>
       </c>
       <c r="B170">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>UNIVERSITY OF TRENTO</v>
+        <v>AMIRKABIR UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B171">
         <v>26</v>
@@ -1750,18 +1750,18 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>AMIRKABIR UNIVERSITY OF TECHNOLOGY</v>
+        <v>CHANGZHOU UNIVERSITY</v>
       </c>
       <c r="B172">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>CORNELL UNIVERSITY</v>
+        <v>ETH ZURICH</v>
       </c>
       <c r="B173">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="174">
@@ -1769,132 +1769,132 @@
         <v>HOHAI UNIVERSITY</v>
       </c>
       <c r="B174">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>KARLSRUHE INSTITUTE OF TECHNOLOGY</v>
+        <v>ISLAMIC AZAD UNIVERSITY</v>
       </c>
       <c r="B175">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>KU LEUVEN</v>
+        <v>KING FAHD UNIVERSITY OF PETROLEUM MINERALS</v>
       </c>
       <c r="B176">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>STATE UNIVERSITY OF NEW YORK SUNY SYSTEM</v>
+        <v>UNIVERSIDADE DE LISBOA</v>
       </c>
       <c r="B177">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>TORONTO METROPOLITAN UNIVERSITY</v>
+        <v>UNIVERSITAT POLITECNICA DE VALENCIA</v>
       </c>
       <c r="B178">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>UNIVERSIDADE DE LISBOA</v>
+        <v>UNIVERSITE DE MONTREAL</v>
       </c>
       <c r="B179">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>UNIVERSITY OF COLORADO BOULDER</v>
+        <v>UNIVERSITY OF GRONINGEN</v>
       </c>
       <c r="B180">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>UNIVERSITY OF SALERNO</v>
+        <v>UNIVERSITY OF TRENTO</v>
       </c>
       <c r="B181">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>YANGZHOU UNIVERSITY</v>
+        <v>XI AN UNIVERSITY OF ARCHITECTURE TECHNOLOGY</v>
       </c>
       <c r="B182">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>CHINA UNIVERSITY OF GEOSCIENCES</v>
+        <v>CORNELL UNIVERSITY</v>
       </c>
       <c r="B183">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>DEAKIN UNIVERSITY</v>
+        <v>KARLSRUHE INSTITUTE OF TECHNOLOGY</v>
       </c>
       <c r="B184">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>ISLAMIC AZAD UNIVERSITY</v>
+        <v>LAOSHAN LABORATORY</v>
       </c>
       <c r="B185">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>JINAN UNIVERSITY</v>
+        <v>STATE UNIVERSITY OF NEW YORK SUNY SYSTEM</v>
       </c>
       <c r="B186">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>KOREA ADVANCED INSTITUTE OF SCIENCE TECHNOLOGY KAIST</v>
+        <v>TORONTO METROPOLITAN UNIVERSITY</v>
       </c>
       <c r="B187">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>LAOSHAN LABORATORY</v>
+        <v>UNIVERSITY OF COLORADO BOULDER</v>
       </c>
       <c r="B188">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>LEIBNIZ INSTITUT FUR POLYMERFORSCHUNG DRESDEN</v>
+        <v>UNIVERSITY OF SALERNO</v>
       </c>
       <c r="B189">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>LULEA UNIVERSITY OF TECHNOLOGY</v>
+        <v>CHONGQING JIAOTONG UNIVERSITY</v>
       </c>
       <c r="B190">
         <v>24</v>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>ROYAL MELBOURNE INSTITUTE OF TECHNOLOGY RMIT</v>
+        <v>DEAKIN UNIVERSITY</v>
       </c>
       <c r="B191">
         <v>24</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>SUZHOU UNIVERSITY OF SCIENCE TECHNOLOGY</v>
+        <v>JINAN UNIVERSITY</v>
       </c>
       <c r="B192">
         <v>24</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>TAIYUAN UNIVERSITY OF TECHNOLOGY</v>
+        <v>KOREA ADVANCED INSTITUTE OF SCIENCE TECHNOLOGY KAIST</v>
       </c>
       <c r="B193">
         <v>24</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>UNIVERSIDAD DEL BIO BIO</v>
+        <v>LEIBNIZ INSTITUT FUR POLYMERFORSCHUNG DRESDEN</v>
       </c>
       <c r="B194">
         <v>24</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>UNIVERSITAT POLITECNICA DE VALENCIA</v>
+        <v>LULEA UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B195">
         <v>24</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>UNIVERSITE PSL</v>
+        <v>ROYAL MELBOURNE INSTITUTE OF TECHNOLOGY RMIT</v>
       </c>
       <c r="B196">
         <v>24</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>UNIVERSITY OF CALIFORNIA LOS ANGELES</v>
+        <v>SUZHOU UNIVERSITY OF SCIENCE TECHNOLOGY</v>
       </c>
       <c r="B197">
         <v>24</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>XI AN UNIVERSITY OF ARCHITECTURE TECHNOLOGY</v>
+        <v>UNIVERSITE PSL</v>
       </c>
       <c r="B198">
         <v>24</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>ZHEJIANG SCI TECH UNIVERSITY</v>
+        <v>UNIVERSITY OF CALIFORNIA LOS ANGELES</v>
       </c>
       <c r="B199">
         <v>24</v>
@@ -1974,18 +1974,18 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>A STAR INSTITUTE OF MATERIALS RESEARCH ENGINEERING IMRE</v>
+        <v>ZHEJIANG SCI TECH UNIVERSITY</v>
       </c>
       <c r="B200">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>CHANGCHUN UNIVERSITY OF TECHNOLOGY</v>
+        <v>ZHEJIANG UNIVERSITY OF TECHNOLOGY</v>
       </c>
       <c r="B201">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>